<commit_message>
Renamed the spectra graph
</commit_message>
<xml_diff>
--- a/Mare Tranquillitatis_Serenitatis Spectra.xlsx
+++ b/Mare Tranquillitatis_Serenitatis Spectra.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lizzie\MoonSpectroscopy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenter\Dropbox\Aber Uni\Experimental Physics\Lunar\MoonSpectroscopy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -221,12 +221,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="nb-NO"/>
-              <a:t>Mare Tranquillitatis &amp; Serenitatis Albedo Spectra</a:t>
+              <a:t>Mare Tranquillitatis &amp; Serenitatis Spectra</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17721684601058066"/>
+          <c:y val="1.9161669418956324E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -548,11 +555,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="298093288"/>
-        <c:axId val="298092112"/>
+        <c:axId val="116937376"/>
+        <c:axId val="103523936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="298093288"/>
+        <c:axId val="116937376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="400"/>
@@ -652,12 +659,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298092112"/>
+        <c:crossAx val="103523936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="298092112"/>
+        <c:axId val="103523936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.30000000000000004"/>
@@ -701,7 +708,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Reflectivity /% </a:t>
+                  <a:t>Relaitive</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Intesity /% </a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -767,7 +782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="298093288"/>
+        <c:crossAx val="116937376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -818,6 +833,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>

</xml_diff>